<commit_message>
Guías de Uso DAMOP CATALOGOS
</commit_message>
<xml_diff>
--- a/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
+++ b/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github Repositorio\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Iris Lechuga</author>
+  </authors>
+  <commentList>
+    <comment ref="E31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Iris Lechuga:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Estas son de Catalogos Damop </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
   <si>
     <t>CPCH</t>
   </si>
@@ -216,9 +250,6 @@
   </si>
   <si>
     <t>AVISOS</t>
-  </si>
-  <si>
-    <t>CONTACTO MUNICIPIOS</t>
   </si>
   <si>
     <t>PARTICIPACIONES</t>
@@ -422,7 +453,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,8 +492,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,6 +528,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -617,6 +667,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,23 +691,137 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -656,130 +829,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,11 +1110,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,45 +1127,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="B2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>111</v>
-      </c>
       <c r="H3" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="47" t="s">
+      <c r="C4" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1125,9 +1176,9 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="59"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="48"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
@@ -1136,133 +1187,149 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="59"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="59"/>
-      <c r="C7" s="50" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="59"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="59"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="18"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="59"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="59"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="59"/>
-      <c r="C12" s="52" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="39" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="59"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="30"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="59"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="30"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="59"/>
-      <c r="C15" s="15" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="61" t="s">
@@ -1272,241 +1339,269 @@
         <v>13</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" s="12"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="59"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="62"/>
       <c r="E16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" s="12"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="59"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="62"/>
       <c r="E17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="59"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="62"/>
       <c r="E18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="59"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="62"/>
       <c r="E19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="62"/>
       <c r="E20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="59"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="62"/>
       <c r="E21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="59"/>
-      <c r="C22" s="16"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="62"/>
       <c r="E22" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="59"/>
-      <c r="C23" s="16"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="62"/>
       <c r="E23" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="59"/>
-      <c r="C24" s="16"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="62"/>
       <c r="E24" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
-      <c r="C25" s="16"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="62"/>
       <c r="E25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="62"/>
       <c r="E26" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G26" s="12"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
-      <c r="C27" s="16"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="62"/>
       <c r="E27" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="6"/>
+      <c r="H27" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="59"/>
-      <c r="C28" s="16"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="62"/>
       <c r="E28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G28" s="12"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="59"/>
-      <c r="C29" s="16"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="62"/>
       <c r="E29" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="59"/>
-      <c r="C30" s="16"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="62"/>
       <c r="E30" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="31" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="59"/>
-      <c r="C31" s="16"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="62"/>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="67" t="s">
         <v>63</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="59"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="62"/>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="59"/>
-      <c r="C33" s="16"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="62"/>
-      <c r="E33" s="60" t="s">
+      <c r="E33" s="68" t="s">
         <v>60</v>
       </c>
       <c r="F33" s="6"/>
@@ -1514,10 +1609,10 @@
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="59"/>
-      <c r="C34" s="16"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="63"/>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="67" t="s">
         <v>61</v>
       </c>
       <c r="F34" s="6"/>
@@ -1525,57 +1620,57 @@
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="59"/>
-      <c r="C35" s="16"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="59"/>
-      <c r="C36" s="16"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="62"/>
       <c r="E36" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="59"/>
-      <c r="C37" s="16"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="62"/>
       <c r="E37" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="59"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="63"/>
       <c r="E38" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="59"/>
-      <c r="C39" s="31" t="s">
+      <c r="B39" s="37"/>
+      <c r="C39" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="39" t="s">
         <v>1</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1583,71 +1678,83 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="H39" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="59"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="30"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="39"/>
       <c r="E40" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="H40" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="59"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="30"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="39"/>
       <c r="E41" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="H41" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="59"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="30"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="39"/>
       <c r="E42" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="59"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="30"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="39"/>
       <c r="E43" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="H43" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="59"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="30"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="39"/>
       <c r="E44" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="59"/>
-      <c r="C45" s="50" t="s">
+      <c r="B45" s="37"/>
+      <c r="C45" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="D45" s="36" t="s">
         <v>1</v>
       </c>
       <c r="E45" s="6" t="s">
@@ -1655,27 +1762,31 @@
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
+      <c r="H45" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="46" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="59"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="53"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="36"/>
       <c r="E46" s="9" t="s">
         <v>39</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="59"/>
-      <c r="C47" s="50" t="s">
+      <c r="B47" s="37"/>
+      <c r="C47" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="32" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="7" t="s">
@@ -1683,124 +1794,146 @@
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="H47" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="59"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="18"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
+      <c r="H48" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="59"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="18"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="6" t="s">
         <v>43</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="H49" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="59"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="18"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="6" t="s">
         <v>44</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
+      <c r="H50" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="59"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="18"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
+      <c r="H51" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="59"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="18"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
+      <c r="H52" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="59"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="32"/>
       <c r="E53" s="8" t="s">
         <v>46</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
+      <c r="H53" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="59"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="18"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="32"/>
       <c r="E54" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
+      <c r="H54" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="59"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="18"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
+      <c r="H55" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="59"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="18"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="32"/>
       <c r="E56" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
+      <c r="H56" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="57" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="59"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="18"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
+      <c r="H57" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="58" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B58" s="59"/>
-      <c r="C58" s="52" t="s">
+      <c r="B58" s="37"/>
+      <c r="C58" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="51" t="s">
+      <c r="D58" s="34" t="s">
         <v>10</v>
       </c>
       <c r="E58" s="4" t="s">
@@ -1808,27 +1941,31 @@
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
+      <c r="H58" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="59" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="59"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="51"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="34"/>
       <c r="E59" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
+      <c r="H59" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="23" t="s">
         <v>56</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -1839,9 +1976,9 @@
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="26"/>
+      <c r="B61" s="13"/>
       <c r="C61" s="64"/>
-      <c r="D61" s="22"/>
+      <c r="D61" s="24"/>
       <c r="E61" s="1" t="s">
         <v>52</v>
       </c>
@@ -1850,9 +1987,9 @@
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="26"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="23"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="25"/>
       <c r="E62" s="2" t="s">
         <v>57</v>
       </c>
@@ -1861,13 +1998,13 @@
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="31" t="s">
+      <c r="B63" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="D63" s="24" t="s">
+      <c r="C63" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="65" t="s">
         <v>59</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -1878,9 +2015,9 @@
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="31"/>
-      <c r="C64" s="66"/>
-      <c r="D64" s="25"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="53"/>
+      <c r="D64" s="66"/>
       <c r="E64" s="5" t="s">
         <v>52</v>
       </c>
@@ -1889,11 +2026,11 @@
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="31"/>
-      <c r="C65" s="31" t="s">
+      <c r="B65" s="38"/>
+      <c r="C65" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="39" t="s">
         <v>59</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -1901,131 +2038,143 @@
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
+      <c r="H65" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="31"/>
-      <c r="C66" s="31"/>
-      <c r="D66" s="30"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="39"/>
       <c r="E66" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
+      <c r="H66" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="30"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="39"/>
       <c r="E67" s="3" t="s">
         <v>61</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
+      <c r="H67" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="30"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="39"/>
       <c r="E68" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
+      <c r="H68" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="30"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="39"/>
       <c r="E69" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
+      <c r="H69" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="30"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="39"/>
       <c r="E70" s="3" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
+      <c r="H70" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="31"/>
-      <c r="C71" s="31" t="s">
+      <c r="B71" s="38"/>
+      <c r="C71" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D71" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D71" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="31"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="30"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="39"/>
       <c r="E72" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="31"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="30"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="39"/>
       <c r="E73" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="31"/>
-      <c r="C74" s="31"/>
-      <c r="D74" s="30"/>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="39"/>
       <c r="E74" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="31"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="30"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="39"/>
       <c r="E75" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="26" t="s">
+      <c r="B76" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D76" s="43" t="s">
         <v>71</v>
-      </c>
-      <c r="C76" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D76" s="35" t="s">
-        <v>72</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>52</v>
@@ -2035,83 +2184,83 @@
       <c r="H76" s="1"/>
     </row>
     <row r="77" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="26"/>
-      <c r="C77" s="41"/>
-      <c r="D77" s="36"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="44"/>
       <c r="E77" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="31" t="s">
+      <c r="B78" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" s="40"/>
+      <c r="D78" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="C78" s="32"/>
-      <c r="D78" s="54" t="s">
+      <c r="E78" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="31"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="55"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="41"/>
+      <c r="D79" s="46"/>
       <c r="E79" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="31"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="55"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="46"/>
       <c r="E80" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="31"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="55"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="46"/>
       <c r="E81" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="31"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="55"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="41"/>
+      <c r="D82" s="46"/>
       <c r="E82" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="31"/>
-      <c r="C83" s="34"/>
-      <c r="D83" s="56"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="47"/>
       <c r="E83" s="5" t="s">
         <v>52</v>
       </c>
@@ -2120,38 +2269,38 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="57"/>
-      <c r="C84" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="D84" s="42" t="s">
+      <c r="B84" s="56"/>
+      <c r="C84" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="58"/>
-      <c r="C85" s="41"/>
-      <c r="D85" s="43"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="55"/>
       <c r="E85" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="C86" s="27"/>
-      <c r="D86" s="21" t="s">
-        <v>117</v>
+      <c r="B86" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C86" s="58"/>
+      <c r="D86" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>52</v>
@@ -2161,9 +2310,9 @@
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="26"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="22"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="59"/>
+      <c r="D87" s="24"/>
       <c r="E87" s="1" t="s">
         <v>53</v>
       </c>
@@ -2172,25 +2321,25 @@
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="26"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="23"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="60"/>
+      <c r="D88" s="25"/>
       <c r="E88" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C89" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="D89" s="30" t="s">
-        <v>118</v>
+      <c r="B89" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D89" s="39" t="s">
+        <v>117</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>53</v>
@@ -2200,94 +2349,96 @@
       <c r="H89" s="3"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="38"/>
-      <c r="C90" s="67"/>
-      <c r="D90" s="30"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="39"/>
       <c r="E90" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="38"/>
-      <c r="C91" s="67"/>
-      <c r="D91" s="30"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="52"/>
+      <c r="D91" s="39"/>
       <c r="E91" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="38"/>
-      <c r="C92" s="67"/>
-      <c r="D92" s="30"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="52"/>
+      <c r="D92" s="39"/>
       <c r="E92" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="38"/>
-      <c r="C93" s="67"/>
-      <c r="D93" s="30"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="52"/>
+      <c r="D93" s="39"/>
       <c r="E93" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="38"/>
-      <c r="C94" s="67"/>
-      <c r="D94" s="30"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="52"/>
+      <c r="D94" s="39"/>
       <c r="E94" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="38"/>
-      <c r="C95" s="67"/>
-      <c r="D95" s="30"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="52"/>
+      <c r="D95" s="39"/>
       <c r="E95" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="39"/>
-      <c r="C96" s="66"/>
-      <c r="D96" s="30"/>
+      <c r="B96" s="50"/>
+      <c r="C96" s="53"/>
+      <c r="D96" s="39"/>
       <c r="E96" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D7:D11"/>
     <mergeCell ref="D15:D34"/>
     <mergeCell ref="D35:D38"/>
     <mergeCell ref="C7:C11"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D39:D44"/>
     <mergeCell ref="D89:D96"/>
     <mergeCell ref="B89:B96"/>
     <mergeCell ref="C89:C96"/>
@@ -2295,9 +2446,6 @@
     <mergeCell ref="D84:D85"/>
     <mergeCell ref="B84:B85"/>
     <mergeCell ref="D86:D88"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
     <mergeCell ref="B86:B88"/>
     <mergeCell ref="C86:C88"/>
     <mergeCell ref="D71:D75"/>
@@ -2308,6 +2456,8 @@
     <mergeCell ref="C78:C83"/>
     <mergeCell ref="D76:D77"/>
     <mergeCell ref="D78:D83"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="C65:C70"/>
     <mergeCell ref="B60:B62"/>
     <mergeCell ref="C76:C77"/>
     <mergeCell ref="B2:H2"/>
@@ -2324,9 +2474,9 @@
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="B4:B59"/>
     <mergeCell ref="C39:C44"/>
-    <mergeCell ref="D7:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización Matriz de guías CPH
</commit_message>
<xml_diff>
--- a/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
+++ b/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github Repositorio\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\menu\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUCIONES" sheetId="1" r:id="rId1"/>
@@ -705,170 +705,170 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,39 +1152,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+    </row>
+    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="28"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="10" t="s">
         <v>106</v>
       </c>
@@ -1198,14 +1198,14 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1217,10 +1217,10 @@
       <c r="G4" s="12"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="44"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="36"/>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="40"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1230,10 +1230,10 @@
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="37"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="40"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
@@ -1243,12 +1243,12 @@
       <c r="G6" s="15"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
-      <c r="C7" s="40" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="40"/>
+      <c r="C7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="16" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1262,10 +1262,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="70"/>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="40"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1277,10 +1277,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="70"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="40"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
@@ -1292,10 +1292,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="70"/>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="40"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="6" t="s">
         <v>95</v>
       </c>
@@ -1307,10 +1307,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="44"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="70"/>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="40"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1322,12 +1322,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="38" t="s">
+    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
+      <c r="C12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1336,47 +1336,47 @@
       <c r="F12" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="44"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="19"/>
+    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="40"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="44"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="19"/>
+    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="40"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="44"/>
-      <c r="C15" s="25" t="s">
+    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="40"/>
+      <c r="C15" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1390,10 +1390,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="44"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="60"/>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="40"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1405,10 +1405,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="44"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="60"/>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="40"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1422,10 +1422,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="44"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="60"/>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="40"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1437,10 +1437,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="44"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="60"/>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="40"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1452,10 +1452,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="44"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="60"/>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="40"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1467,10 +1467,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="60"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="40"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1482,10 +1482,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="44"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="60"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="40"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1497,10 +1497,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="60"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="40"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1512,10 +1512,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="44"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="60"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="40"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1527,10 +1527,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="44"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="60"/>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="40"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1542,10 +1542,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="44"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="60"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="40"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="6" t="s">
         <v>118</v>
       </c>
@@ -1557,10 +1557,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="44"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="60"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="40"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1572,10 +1572,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="60"/>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="40"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1587,10 +1587,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="60"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="40"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="6" t="s">
         <v>24</v>
       </c>
@@ -1602,10 +1602,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="44"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="60"/>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="40"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1617,12 +1617,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="44"/>
-      <c r="C31" s="20" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="40"/>
+      <c r="C31" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1636,10 +1636,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="44"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="19"/>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="40"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1651,10 +1651,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="44"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="19"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="40"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="20"/>
       <c r="E33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1666,10 +1666,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="44"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="19"/>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="40"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="3" t="s">
         <v>31</v>
       </c>
@@ -1681,10 +1681,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="44"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="19"/>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="40"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="3" t="s">
         <v>32</v>
       </c>
@@ -1696,10 +1696,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="44"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="19"/>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="40"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="3" t="s">
         <v>123</v>
       </c>
@@ -1709,10 +1709,10 @@
       <c r="G36" s="12"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="44"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="19"/>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="40"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="3" t="s">
         <v>121</v>
       </c>
@@ -1722,10 +1722,10 @@
       <c r="G37" s="12"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="44"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="19"/>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="40"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="3" t="s">
         <v>122</v>
       </c>
@@ -1735,10 +1735,10 @@
       <c r="G38" s="12"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="44"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="19"/>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="40"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="3" t="s">
         <v>97</v>
       </c>
@@ -1750,223 +1750,223 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="44"/>
-      <c r="C40" s="40" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="40"/>
+      <c r="C40" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="67" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="44"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="41"/>
+    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="40"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G41" s="9"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="44"/>
-      <c r="C42" s="38" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="40"/>
+      <c r="C42" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="44"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="19"/>
+    <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="40"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="20"/>
       <c r="E43" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="G43" s="12"/>
       <c r="H43" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="44"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="19"/>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="40"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
+      <c r="G44" s="12"/>
       <c r="H44" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="44"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="19"/>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="40"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="12"/>
       <c r="H45" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="44"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="19"/>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="40"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="12"/>
       <c r="H46" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="44"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="19"/>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="40"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="12"/>
       <c r="H47" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="44"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="19"/>
+    <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="40"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="12"/>
       <c r="H48" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="44"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="19"/>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="40"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="20"/>
       <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="44"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="19"/>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="40"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="20"/>
       <c r="E50" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
+      <c r="G50" s="12"/>
       <c r="H50" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="44"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="19"/>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="40"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="20"/>
       <c r="E51" s="3" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="12"/>
       <c r="H51" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="44"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="19"/>
+    <row r="52" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B52" s="40"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="20"/>
       <c r="E52" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
+      <c r="G52" s="12"/>
       <c r="H52" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="44"/>
-      <c r="C53" s="40" t="s">
+    <row r="53" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="40"/>
+      <c r="C53" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="39" t="s">
+      <c r="D53" s="66" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+      <c r="G53" s="12"/>
       <c r="H53" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="45"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="39"/>
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="41"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="66"/>
       <c r="E54" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
+      <c r="G54" s="12"/>
       <c r="H54" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="16" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D55" s="47" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -1976,10 +1976,10 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="16"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="30"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="50"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1987,10 +1987,10 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="16"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="31"/>
+    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="50"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="49"/>
       <c r="E57" s="2" t="s">
         <v>56</v>
       </c>
@@ -2000,14 +2000,14 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="20" t="s">
+    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="49" t="s">
+      <c r="C58" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="D58" s="68" t="s">
+      <c r="D58" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -2017,10 +2017,10 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="20"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="69"/>
+    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="22"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
@@ -2028,12 +2028,12 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="20"/>
-      <c r="C60" s="20" t="s">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B60" s="22"/>
+      <c r="C60" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="D60" s="20" t="s">
         <v>58</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2045,10 +2045,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="19"/>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="20"/>
       <c r="E61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2058,10 +2058,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="19"/>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="20"/>
       <c r="E62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2071,10 +2071,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="19"/>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="20"/>
       <c r="E63" s="3" t="s">
         <v>61</v>
       </c>
@@ -2084,10 +2084,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="19"/>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="3" t="s">
         <v>22</v>
       </c>
@@ -2097,10 +2097,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="19"/>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="20"/>
       <c r="E65" s="3" t="s">
         <v>100</v>
       </c>
@@ -2110,12 +2110,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="20"/>
-      <c r="C66" s="20" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B66" s="22"/>
+      <c r="C66" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="D66" s="20" t="s">
         <v>58</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2125,10 +2125,10 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="19"/>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="20"/>
       <c r="E67" s="3" t="s">
         <v>65</v>
       </c>
@@ -2136,10 +2136,10 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="19"/>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="20"/>
       <c r="E68" s="3" t="s">
         <v>66</v>
       </c>
@@ -2147,10 +2147,10 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="19"/>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="20"/>
       <c r="E69" s="3" t="s">
         <v>67</v>
       </c>
@@ -2158,10 +2158,10 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="19"/>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="20"/>
       <c r="E70" s="3" t="s">
         <v>68</v>
       </c>
@@ -2169,14 +2169,14 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="16" t="s">
+    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="C71" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="21" t="s">
+      <c r="D71" s="69" t="s">
         <v>70</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -2186,10 +2186,10 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="16"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="22"/>
+    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="50"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="70"/>
       <c r="E72" s="2" t="s">
         <v>71</v>
       </c>
@@ -2197,12 +2197,12 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="20" t="s">
+    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="62"/>
-      <c r="D73" s="65" t="s">
+      <c r="C73" s="23"/>
+      <c r="D73" s="26" t="s">
         <v>73</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2214,10 +2214,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="20"/>
-      <c r="C74" s="63"/>
-      <c r="D74" s="66"/>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B74" s="22"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="27"/>
       <c r="E74" s="3" t="s">
         <v>75</v>
       </c>
@@ -2229,10 +2229,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
-      <c r="C75" s="63"/>
-      <c r="D75" s="66"/>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" s="22"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="27"/>
       <c r="E75" s="3" t="s">
         <v>76</v>
       </c>
@@ -2242,10 +2242,10 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="20"/>
-      <c r="C76" s="63"/>
-      <c r="D76" s="66"/>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B76" s="22"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="27"/>
       <c r="E76" s="3" t="s">
         <v>77</v>
       </c>
@@ -2253,10 +2253,10 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="20"/>
-      <c r="C77" s="63"/>
-      <c r="D77" s="66"/>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B77" s="22"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="27"/>
       <c r="E77" s="3" t="s">
         <v>78</v>
       </c>
@@ -2264,10 +2264,10 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="20"/>
-      <c r="C78" s="64"/>
-      <c r="D78" s="67"/>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B78" s="22"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="28"/>
       <c r="E78" s="5" t="s">
         <v>51</v>
       </c>
@@ -2275,12 +2275,12 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="43" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79" s="39" t="s">
         <v>22</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="59" t="s">
+      <c r="D79" s="17" t="s">
         <v>112</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -2294,10 +2294,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="44"/>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B80" s="40"/>
       <c r="C80" s="13"/>
-      <c r="D80" s="60"/>
+      <c r="D80" s="18"/>
       <c r="E80" s="6" t="s">
         <v>100</v>
       </c>
@@ -2309,10 +2309,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="44"/>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B81" s="40"/>
       <c r="C81" s="13"/>
-      <c r="D81" s="60"/>
+      <c r="D81" s="18"/>
       <c r="E81" s="14" t="s">
         <v>59</v>
       </c>
@@ -2322,10 +2322,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="44"/>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B82" s="40"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="60"/>
+      <c r="D82" s="18"/>
       <c r="E82" s="6" t="s">
         <v>60</v>
       </c>
@@ -2335,10 +2335,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="44"/>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B83" s="40"/>
       <c r="C83" s="13"/>
-      <c r="D83" s="60"/>
+      <c r="D83" s="18"/>
       <c r="E83" s="6" t="s">
         <v>83</v>
       </c>
@@ -2348,10 +2348,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="44"/>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B84" s="40"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="60"/>
+      <c r="D84" s="18"/>
       <c r="E84" s="6" t="s">
         <v>84</v>
       </c>
@@ -2361,10 +2361,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="44"/>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B85" s="40"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="60"/>
+      <c r="D85" s="18"/>
       <c r="E85" s="6" t="s">
         <v>85</v>
       </c>
@@ -2372,10 +2372,10 @@
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="45"/>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B86" s="41"/>
       <c r="C86" s="13"/>
-      <c r="D86" s="61"/>
+      <c r="D86" s="42"/>
       <c r="E86" s="6" t="s">
         <v>86</v>
       </c>
@@ -2383,12 +2383,12 @@
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
     </row>
-    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="57"/>
-      <c r="C87" s="17" t="s">
+    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="37"/>
+      <c r="C87" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="D87" s="55" t="s">
+      <c r="D87" s="33" t="s">
         <v>79</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -2398,10 +2398,10 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="58"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="56"/>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B88" s="38"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="34"/>
       <c r="E88" s="1" t="s">
         <v>81</v>
       </c>
@@ -2409,12 +2409,12 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="16" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B89" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="52"/>
-      <c r="D89" s="29" t="s">
+      <c r="C89" s="51"/>
+      <c r="D89" s="47" t="s">
         <v>113</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -2424,10 +2424,10 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="16"/>
-      <c r="C90" s="53"/>
-      <c r="D90" s="30"/>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B90" s="50"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="1" t="s">
         <v>52</v>
       </c>
@@ -2435,10 +2435,10 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="16"/>
-      <c r="C91" s="54"/>
-      <c r="D91" s="31"/>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B91" s="50"/>
+      <c r="C91" s="53"/>
+      <c r="D91" s="49"/>
       <c r="E91" s="2" t="s">
         <v>84</v>
       </c>
@@ -2446,14 +2446,14 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="46" t="s">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B92" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="49" t="s">
+      <c r="C92" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D92" s="20" t="s">
         <v>114</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -2463,10 +2463,10 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="47"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="19"/>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B93" s="44"/>
+      <c r="C93" s="46"/>
+      <c r="D93" s="20"/>
       <c r="E93" s="15" t="s">
         <v>88</v>
       </c>
@@ -2474,10 +2474,10 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="47"/>
-      <c r="C94" s="50"/>
-      <c r="D94" s="19"/>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B94" s="44"/>
+      <c r="C94" s="46"/>
+      <c r="D94" s="20"/>
       <c r="E94" s="15" t="s">
         <v>89</v>
       </c>
@@ -2485,10 +2485,10 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="47"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="19"/>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B95" s="44"/>
+      <c r="C95" s="46"/>
+      <c r="D95" s="20"/>
       <c r="E95" s="15" t="s">
         <v>90</v>
       </c>
@@ -2496,10 +2496,10 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="47"/>
-      <c r="C96" s="50"/>
-      <c r="D96" s="19"/>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B96" s="44"/>
+      <c r="C96" s="46"/>
+      <c r="D96" s="20"/>
       <c r="E96" s="15" t="s">
         <v>91</v>
       </c>
@@ -2507,10 +2507,10 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="47"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="19"/>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B97" s="44"/>
+      <c r="C97" s="46"/>
+      <c r="D97" s="20"/>
       <c r="E97" s="15" t="s">
         <v>92</v>
       </c>
@@ -2518,10 +2518,10 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="47"/>
-      <c r="C98" s="50"/>
-      <c r="D98" s="19"/>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B98" s="44"/>
+      <c r="C98" s="46"/>
+      <c r="D98" s="20"/>
       <c r="E98" s="15" t="s">
         <v>93</v>
       </c>
@@ -2529,10 +2529,10 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="48"/>
-      <c r="C99" s="51"/>
-      <c r="D99" s="19"/>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B99" s="45"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="20"/>
       <c r="E99" s="3" t="s">
         <v>94</v>
       </c>
@@ -2544,27 +2544,15 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D15:D30"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="D73:D78"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B79:B86"/>
-    <mergeCell ref="D79:D86"/>
-    <mergeCell ref="D92:D99"/>
-    <mergeCell ref="B92:B99"/>
-    <mergeCell ref="C92:C99"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="B58:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="C60:C65"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C15:C30"/>
     <mergeCell ref="C3:D3"/>
@@ -2581,15 +2569,27 @@
     <mergeCell ref="D31:D39"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="B4:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="B58:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="D92:D99"/>
+    <mergeCell ref="B92:B99"/>
+    <mergeCell ref="C92:C99"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B79:B86"/>
+    <mergeCell ref="D79:D86"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D15:D30"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización de Matriz de guías
</commit_message>
<xml_diff>
--- a/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
+++ b/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
@@ -705,170 +705,170 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1167,24 +1167,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="59"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="10" t="s">
         <v>106</v>
       </c>
@@ -1199,13 +1199,13 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="35" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1218,9 +1218,9 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="40"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="64"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1231,9 +1231,9 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="40"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="65"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
@@ -1244,11 +1244,11 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="40"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="70" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1257,77 +1257,77 @@
       <c r="F7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="40"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="40"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="70"/>
       <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="40"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="40"/>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1342,9 +1342,9 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="40"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="20"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1357,9 +1357,9 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="20"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1372,11 +1372,11 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="40"/>
-      <c r="C15" s="56" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="59" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1391,9 +1391,9 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="40"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1406,9 +1406,9 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="40"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="18"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1423,9 +1423,9 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="40"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1438,9 +1438,9 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="40"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="18"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1453,9 +1453,9 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1468,9 +1468,9 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="40"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1483,9 +1483,9 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="60"/>
       <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1498,9 +1498,9 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="40"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="18"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="60"/>
       <c r="E23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1513,9 +1513,9 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="40"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="18"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="60"/>
       <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1528,9 +1528,9 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="40"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="18"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="60"/>
       <c r="E25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1543,9 +1543,9 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="40"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="60"/>
       <c r="E26" s="6" t="s">
         <v>118</v>
       </c>
@@ -1558,9 +1558,9 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="40"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="60"/>
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1573,9 +1573,9 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="40"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1588,9 +1588,9 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="40"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="6" t="s">
         <v>24</v>
       </c>
@@ -1603,9 +1603,9 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="40"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="60"/>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1618,11 +1618,11 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="40"/>
-      <c r="C31" s="22" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1637,9 +1637,9 @@
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="40"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="20"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1652,9 +1652,9 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="40"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="20"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1667,9 +1667,9 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="40"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="20"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="3" t="s">
         <v>31</v>
       </c>
@@ -1682,9 +1682,9 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="40"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="20"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="3" t="s">
         <v>32</v>
       </c>
@@ -1697,9 +1697,9 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="40"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="20"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="3" t="s">
         <v>123</v>
       </c>
@@ -1710,9 +1710,9 @@
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="40"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="20"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="3" t="s">
         <v>121</v>
       </c>
@@ -1723,9 +1723,9 @@
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="40"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="20"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="3" t="s">
         <v>122</v>
       </c>
@@ -1736,9 +1736,9 @@
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="40"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="20"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="3" t="s">
         <v>97</v>
       </c>
@@ -1751,11 +1751,11 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="40"/>
-      <c r="C40" s="19" t="s">
+      <c r="B40" s="44"/>
+      <c r="C40" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="67" t="s">
+      <c r="D40" s="41" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
@@ -1768,9 +1768,9 @@
       </c>
     </row>
     <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="40"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="67"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="41"/>
       <c r="E41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1783,11 +1783,11 @@
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="40"/>
-      <c r="C42" s="21" t="s">
+      <c r="B42" s="44"/>
+      <c r="C42" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -1800,9 +1800,9 @@
       </c>
     </row>
     <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B43" s="40"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="20"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1813,9 +1813,9 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="40"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="20"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="3" t="s">
         <v>42</v>
       </c>
@@ -1826,9 +1826,9 @@
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="40"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="20"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="3" t="s">
         <v>43</v>
       </c>
@@ -1839,9 +1839,9 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="40"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="20"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="19"/>
       <c r="E46" s="3" t="s">
         <v>44</v>
       </c>
@@ -1852,9 +1852,9 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="40"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="20"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="19"/>
       <c r="E47" s="3" t="s">
         <v>49</v>
       </c>
@@ -1865,9 +1865,9 @@
       </c>
     </row>
     <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" s="40"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="20"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="19"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
       </c>
@@ -1878,9 +1878,9 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="40"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="20"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="19"/>
       <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
@@ -1891,9 +1891,9 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="40"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="20"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="19"/>
       <c r="E50" s="3" t="s">
         <v>47</v>
       </c>
@@ -1904,9 +1904,9 @@
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="40"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="20"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="19"/>
       <c r="E51" s="3" t="s">
         <v>48</v>
       </c>
@@ -1917,9 +1917,9 @@
       </c>
     </row>
     <row r="52" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B52" s="40"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="20"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="19"/>
       <c r="E52" s="4" t="s">
         <v>50</v>
       </c>
@@ -1930,11 +1930,11 @@
       </c>
     </row>
     <row r="53" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="40"/>
-      <c r="C53" s="19" t="s">
+      <c r="B53" s="44"/>
+      <c r="C53" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="66" t="s">
+      <c r="D53" s="39" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -1947,9 +1947,9 @@
       </c>
     </row>
     <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="41"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="66"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="39"/>
       <c r="E54" s="7" t="s">
         <v>37</v>
       </c>
@@ -1960,13 +1960,13 @@
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D55" s="47" t="s">
+      <c r="D55" s="29" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -1977,9 +1977,9 @@
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B56" s="50"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="48"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1988,9 +1988,9 @@
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="50"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="49"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="2" t="s">
         <v>56</v>
       </c>
@@ -2001,13 +2001,13 @@
       </c>
     </row>
     <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="68" t="s">
         <v>58</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -2018,9 +2018,9 @@
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="22"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="32"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="69"/>
       <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
@@ -2029,11 +2029,11 @@
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B60" s="22"/>
-      <c r="C60" s="22" t="s">
+      <c r="B60" s="20"/>
+      <c r="C60" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="20" t="s">
+      <c r="D60" s="19" t="s">
         <v>58</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2046,9 +2046,9 @@
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="20"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="19"/>
       <c r="E61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2059,9 +2059,9 @@
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="20"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="19"/>
       <c r="E62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2072,9 +2072,9 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B63" s="22"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="20"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="19"/>
       <c r="E63" s="3" t="s">
         <v>61</v>
       </c>
@@ -2085,9 +2085,9 @@
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B64" s="22"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="20"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="19"/>
       <c r="E64" s="3" t="s">
         <v>22</v>
       </c>
@@ -2098,9 +2098,9 @@
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="19"/>
       <c r="E65" s="3" t="s">
         <v>100</v>
       </c>
@@ -2111,11 +2111,11 @@
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B66" s="22"/>
-      <c r="C66" s="22" t="s">
+      <c r="B66" s="20"/>
+      <c r="C66" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="19" t="s">
         <v>58</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2126,9 +2126,9 @@
       <c r="H66" s="3"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="20"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="19"/>
       <c r="E67" s="3" t="s">
         <v>65</v>
       </c>
@@ -2137,9 +2137,9 @@
       <c r="H67" s="3"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="20"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="19"/>
       <c r="E68" s="3" t="s">
         <v>66</v>
       </c>
@@ -2148,9 +2148,9 @@
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="19"/>
       <c r="E69" s="3" t="s">
         <v>67</v>
       </c>
@@ -2159,9 +2159,9 @@
       <c r="H69" s="3"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="19"/>
       <c r="E70" s="3" t="s">
         <v>68</v>
       </c>
@@ -2170,13 +2170,13 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="50" t="s">
+      <c r="B71" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="35" t="s">
+      <c r="C71" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="69" t="s">
+      <c r="D71" s="21" t="s">
         <v>70</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -2187,9 +2187,9 @@
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="50"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="70"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="22"/>
       <c r="E72" s="2" t="s">
         <v>71</v>
       </c>
@@ -2198,11 +2198,11 @@
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="26" t="s">
+      <c r="C73" s="62"/>
+      <c r="D73" s="65" t="s">
         <v>73</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2215,9 +2215,9 @@
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B74" s="22"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="27"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="66"/>
       <c r="E74" s="3" t="s">
         <v>75</v>
       </c>
@@ -2230,9 +2230,9 @@
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B75" s="22"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="27"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="66"/>
       <c r="E75" s="3" t="s">
         <v>76</v>
       </c>
@@ -2243,9 +2243,9 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B76" s="22"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="27"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="66"/>
       <c r="E76" s="3" t="s">
         <v>77</v>
       </c>
@@ -2254,9 +2254,9 @@
       <c r="H76" s="3"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B77" s="22"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="27"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="66"/>
       <c r="E77" s="3" t="s">
         <v>78</v>
       </c>
@@ -2265,9 +2265,9 @@
       <c r="H77" s="3"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B78" s="22"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="28"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="67"/>
       <c r="E78" s="5" t="s">
         <v>51</v>
       </c>
@@ -2276,11 +2276,11 @@
       <c r="H78" s="3"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B79" s="39" t="s">
+      <c r="B79" s="43" t="s">
         <v>22</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="17" t="s">
+      <c r="D79" s="59" t="s">
         <v>112</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -2295,9 +2295,9 @@
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B80" s="40"/>
+      <c r="B80" s="44"/>
       <c r="C80" s="13"/>
-      <c r="D80" s="18"/>
+      <c r="D80" s="60"/>
       <c r="E80" s="6" t="s">
         <v>100</v>
       </c>
@@ -2310,9 +2310,9 @@
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B81" s="40"/>
+      <c r="B81" s="44"/>
       <c r="C81" s="13"/>
-      <c r="D81" s="18"/>
+      <c r="D81" s="60"/>
       <c r="E81" s="14" t="s">
         <v>59</v>
       </c>
@@ -2323,9 +2323,9 @@
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B82" s="40"/>
+      <c r="B82" s="44"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="18"/>
+      <c r="D82" s="60"/>
       <c r="E82" s="6" t="s">
         <v>60</v>
       </c>
@@ -2336,9 +2336,9 @@
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B83" s="40"/>
+      <c r="B83" s="44"/>
       <c r="C83" s="13"/>
-      <c r="D83" s="18"/>
+      <c r="D83" s="60"/>
       <c r="E83" s="6" t="s">
         <v>83</v>
       </c>
@@ -2349,9 +2349,9 @@
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B84" s="40"/>
+      <c r="B84" s="44"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="18"/>
+      <c r="D84" s="60"/>
       <c r="E84" s="6" t="s">
         <v>84</v>
       </c>
@@ -2362,9 +2362,9 @@
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B85" s="40"/>
+      <c r="B85" s="44"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="18"/>
+      <c r="D85" s="60"/>
       <c r="E85" s="6" t="s">
         <v>85</v>
       </c>
@@ -2373,9 +2373,9 @@
       <c r="H85" s="6"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B86" s="41"/>
+      <c r="B86" s="45"/>
       <c r="C86" s="13"/>
-      <c r="D86" s="42"/>
+      <c r="D86" s="61"/>
       <c r="E86" s="6" t="s">
         <v>86</v>
       </c>
@@ -2384,11 +2384,11 @@
       <c r="H86" s="6"/>
     </row>
     <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="37"/>
-      <c r="C87" s="35" t="s">
+      <c r="B87" s="57"/>
+      <c r="C87" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D87" s="33" t="s">
+      <c r="D87" s="55" t="s">
         <v>79</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -2399,9 +2399,9 @@
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B88" s="38"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="34"/>
+      <c r="B88" s="58"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="56"/>
       <c r="E88" s="1" t="s">
         <v>81</v>
       </c>
@@ -2410,11 +2410,11 @@
       <c r="H88" s="1"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B89" s="50" t="s">
+      <c r="B89" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="51"/>
-      <c r="D89" s="47" t="s">
+      <c r="C89" s="52"/>
+      <c r="D89" s="29" t="s">
         <v>113</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -2425,9 +2425,9 @@
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B90" s="50"/>
-      <c r="C90" s="52"/>
-      <c r="D90" s="48"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="53"/>
+      <c r="D90" s="30"/>
       <c r="E90" s="1" t="s">
         <v>52</v>
       </c>
@@ -2436,9 +2436,9 @@
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B91" s="50"/>
-      <c r="C91" s="53"/>
-      <c r="D91" s="49"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="54"/>
+      <c r="D91" s="31"/>
       <c r="E91" s="2" t="s">
         <v>84</v>
       </c>
@@ -2447,13 +2447,13 @@
       <c r="H91" s="1"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B92" s="43" t="s">
+      <c r="B92" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="29" t="s">
+      <c r="C92" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="D92" s="20" t="s">
+      <c r="D92" s="19" t="s">
         <v>114</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -2464,9 +2464,9 @@
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B93" s="44"/>
-      <c r="C93" s="46"/>
-      <c r="D93" s="20"/>
+      <c r="B93" s="47"/>
+      <c r="C93" s="50"/>
+      <c r="D93" s="19"/>
       <c r="E93" s="15" t="s">
         <v>88</v>
       </c>
@@ -2475,9 +2475,9 @@
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B94" s="44"/>
-      <c r="C94" s="46"/>
-      <c r="D94" s="20"/>
+      <c r="B94" s="47"/>
+      <c r="C94" s="50"/>
+      <c r="D94" s="19"/>
       <c r="E94" s="15" t="s">
         <v>89</v>
       </c>
@@ -2486,9 +2486,9 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B95" s="44"/>
-      <c r="C95" s="46"/>
-      <c r="D95" s="20"/>
+      <c r="B95" s="47"/>
+      <c r="C95" s="50"/>
+      <c r="D95" s="19"/>
       <c r="E95" s="15" t="s">
         <v>90</v>
       </c>
@@ -2497,9 +2497,9 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B96" s="44"/>
-      <c r="C96" s="46"/>
-      <c r="D96" s="20"/>
+      <c r="B96" s="47"/>
+      <c r="C96" s="50"/>
+      <c r="D96" s="19"/>
       <c r="E96" s="15" t="s">
         <v>91</v>
       </c>
@@ -2508,9 +2508,9 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B97" s="44"/>
-      <c r="C97" s="46"/>
-      <c r="D97" s="20"/>
+      <c r="B97" s="47"/>
+      <c r="C97" s="50"/>
+      <c r="D97" s="19"/>
       <c r="E97" s="15" t="s">
         <v>92</v>
       </c>
@@ -2519,9 +2519,9 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B98" s="44"/>
-      <c r="C98" s="46"/>
-      <c r="D98" s="20"/>
+      <c r="B98" s="47"/>
+      <c r="C98" s="50"/>
+      <c r="D98" s="19"/>
       <c r="E98" s="15" t="s">
         <v>93</v>
       </c>
@@ -2530,9 +2530,9 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B99" s="45"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="20"/>
+      <c r="B99" s="48"/>
+      <c r="C99" s="51"/>
+      <c r="D99" s="19"/>
       <c r="E99" s="3" t="s">
         <v>94</v>
       </c>
@@ -2544,15 +2544,27 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="B58:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D15:D30"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B79:B86"/>
+    <mergeCell ref="D79:D86"/>
+    <mergeCell ref="D92:D99"/>
+    <mergeCell ref="B92:B99"/>
+    <mergeCell ref="C92:C99"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C15:C30"/>
     <mergeCell ref="C3:D3"/>
@@ -2569,27 +2581,15 @@
     <mergeCell ref="D31:D39"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="B4:B54"/>
-    <mergeCell ref="D92:D99"/>
-    <mergeCell ref="B92:B99"/>
-    <mergeCell ref="C92:C99"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B79:B86"/>
-    <mergeCell ref="D79:D86"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="D73:D78"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D15:D30"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="B58:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="C60:C65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización Matriz de Guías PDRMYOP
</commit_message>
<xml_diff>
--- a/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
+++ b/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
@@ -23,6 +23,65 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Iris Lechuga</author>
+  </authors>
+  <commentList>
+    <comment ref="G72" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Iris Lechuga:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Guía pendiente 
+Aun no se sabe su si va a usar DCCP </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G87" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Iris Lechuga:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Estas Guías se quedan en el repositorio para consulta, no se suben a la plataforma </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="118">
   <si>
@@ -407,7 +466,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +504,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -622,8 +694,122 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -631,17 +817,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,112 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1060,11 +1132,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87:C88"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,24 +1150,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="10" t="s">
         <v>98</v>
       </c>
@@ -1110,13 +1182,13 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1129,9 +1201,9 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="43"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="63"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1142,9 +1214,9 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="64"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
@@ -1155,11 +1227,11 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="47"/>
+      <c r="C7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="71" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1174,9 +1246,9 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1189,9 +1261,9 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="71"/>
       <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
@@ -1204,9 +1276,9 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="6" t="s">
         <v>88</v>
       </c>
@@ -1219,9 +1291,9 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1234,11 +1306,11 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
-      <c r="C12" s="24" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1253,9 +1325,9 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="23"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1268,9 +1340,9 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1283,11 +1355,11 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="43"/>
-      <c r="C15" s="55" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="58" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1302,9 +1374,9 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="21"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="59"/>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1317,9 +1389,9 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="21"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1334,9 +1406,9 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="43"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="21"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="59"/>
       <c r="E18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1349,9 +1421,9 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="43"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="59"/>
       <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1364,9 +1436,9 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="43"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="59"/>
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1379,9 +1451,9 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1394,9 +1466,9 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="43"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="21"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="59"/>
       <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1409,9 +1481,9 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="43"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="59"/>
       <c r="E23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1424,9 +1496,9 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="43"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="21"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="59"/>
       <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1439,9 +1511,9 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="43"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="59"/>
       <c r="E25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1454,9 +1526,9 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="43"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="21"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="6" t="s">
         <v>109</v>
       </c>
@@ -1469,9 +1541,9 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="43"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="59"/>
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1484,9 +1556,9 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="43"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="21"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="59"/>
       <c r="E28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1499,9 +1571,9 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="43"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="21"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="59"/>
       <c r="E29" s="6" t="s">
         <v>24</v>
       </c>
@@ -1514,9 +1586,9 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="43"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="21"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="59"/>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1529,11 +1601,11 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="25" t="s">
+      <c r="B31" s="47"/>
+      <c r="C31" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1548,9 +1620,9 @@
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="43"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="23"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1563,9 +1635,9 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="43"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="23"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1578,9 +1650,9 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="43"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="23"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="3" t="s">
         <v>31</v>
       </c>
@@ -1593,9 +1665,9 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="43"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="23"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="3" t="s">
         <v>32</v>
       </c>
@@ -1608,9 +1680,9 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="23"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="3" t="s">
         <v>114</v>
       </c>
@@ -1621,9 +1693,9 @@
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="43"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="23"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="3" t="s">
         <v>112</v>
       </c>
@@ -1634,9 +1706,9 @@
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="43"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="23"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="3" t="s">
         <v>113</v>
       </c>
@@ -1647,9 +1719,9 @@
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="43"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="23"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="3" t="s">
         <v>90</v>
       </c>
@@ -1662,11 +1734,11 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="43"/>
-      <c r="C40" s="22" t="s">
+      <c r="B40" s="47"/>
+      <c r="C40" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="66" t="s">
+      <c r="D40" s="44" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
@@ -1679,9 +1751,9 @@
       </c>
     </row>
     <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="43"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="66"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="44"/>
       <c r="E41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1694,11 +1766,11 @@
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="43"/>
-      <c r="C42" s="24" t="s">
+      <c r="B42" s="47"/>
+      <c r="C42" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -1711,9 +1783,9 @@
       </c>
     </row>
     <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="43"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="23"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1724,9 +1796,9 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="43"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="23"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="3" t="s">
         <v>42</v>
       </c>
@@ -1737,9 +1809,9 @@
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="43"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="23"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="3" t="s">
         <v>43</v>
       </c>
@@ -1750,9 +1822,9 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="43"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="23"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="22"/>
       <c r="E46" s="3" t="s">
         <v>44</v>
       </c>
@@ -1763,9 +1835,9 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="43"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="23"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="22"/>
       <c r="E47" s="3" t="s">
         <v>49</v>
       </c>
@@ -1776,9 +1848,9 @@
       </c>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="43"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="23"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="22"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
       </c>
@@ -1789,9 +1861,9 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="43"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="23"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
@@ -1802,9 +1874,9 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="43"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="23"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="3" t="s">
         <v>47</v>
       </c>
@@ -1815,9 +1887,9 @@
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="43"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="23"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="22"/>
       <c r="E51" s="3" t="s">
         <v>48</v>
       </c>
@@ -1828,9 +1900,9 @@
       </c>
     </row>
     <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="43"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="23"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="22"/>
       <c r="E52" s="4" t="s">
         <v>50</v>
       </c>
@@ -1841,11 +1913,11 @@
       </c>
     </row>
     <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="43"/>
-      <c r="C53" s="22" t="s">
+      <c r="B53" s="47"/>
+      <c r="C53" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="65" t="s">
+      <c r="D53" s="42" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -1858,9 +1930,9 @@
       </c>
     </row>
     <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="44"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="65"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="42"/>
       <c r="E54" s="7" t="s">
         <v>37</v>
       </c>
@@ -1871,13 +1943,13 @@
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="49" t="s">
+      <c r="B55" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="C55" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="46" t="s">
+      <c r="D55" s="32" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -1888,9 +1960,9 @@
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="49"/>
-      <c r="C56" s="67"/>
-      <c r="D56" s="47"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="33"/>
       <c r="E56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1899,9 +1971,9 @@
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="49"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="48"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="34"/>
       <c r="E57" s="2" t="s">
         <v>56</v>
       </c>
@@ -1912,13 +1984,13 @@
       </c>
     </row>
     <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="32" t="s">
+      <c r="C58" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="D58" s="69" t="s">
         <v>58</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -1929,9 +2001,9 @@
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="25"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="35"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="68"/>
+      <c r="D59" s="70"/>
       <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
@@ -1940,11 +2012,11 @@
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="25"/>
-      <c r="C60" s="25" t="s">
+      <c r="B60" s="23"/>
+      <c r="C60" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="23" t="s">
+      <c r="D60" s="22" t="s">
         <v>58</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -1957,9 +2029,9 @@
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="23"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="22"/>
       <c r="E61" s="3" t="s">
         <v>59</v>
       </c>
@@ -1970,9 +2042,9 @@
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="23"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="22"/>
       <c r="E62" s="3" t="s">
         <v>60</v>
       </c>
@@ -1983,9 +2055,9 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="23"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="22"/>
       <c r="E63" s="3" t="s">
         <v>61</v>
       </c>
@@ -1996,9 +2068,9 @@
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="23"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="22"/>
       <c r="E64" s="3" t="s">
         <v>22</v>
       </c>
@@ -2009,9 +2081,9 @@
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="23"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="22"/>
       <c r="E65" s="3" t="s">
         <v>93</v>
       </c>
@@ -2022,11 +2094,11 @@
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="25"/>
-      <c r="C66" s="25" t="s">
+      <c r="B66" s="23"/>
+      <c r="C66" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="23" t="s">
+      <c r="D66" s="22" t="s">
         <v>58</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2037,9 +2109,9 @@
       <c r="H66" s="3"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="23"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="22"/>
       <c r="E67" s="3" t="s">
         <v>65</v>
       </c>
@@ -2048,9 +2120,9 @@
       <c r="H67" s="3"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="23"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="22"/>
       <c r="E68" s="3" t="s">
         <v>66</v>
       </c>
@@ -2059,9 +2131,9 @@
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="23"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="22"/>
       <c r="E69" s="3" t="s">
         <v>67</v>
       </c>
@@ -2070,9 +2142,9 @@
       <c r="H69" s="3"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="23"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="22"/>
       <c r="E70" s="3" t="s">
         <v>68</v>
       </c>
@@ -2081,13 +2153,13 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="49" t="s">
+      <c r="B71" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="38" t="s">
+      <c r="C71" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D71" s="68" t="s">
+      <c r="D71" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -2098,22 +2170,22 @@
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="49"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="69"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="25"/>
       <c r="E72" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
+      <c r="G72" s="15"/>
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="25" t="s">
+      <c r="B73" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="26"/>
-      <c r="D73" s="29" t="s">
+      <c r="C73" s="61"/>
+      <c r="D73" s="64" t="s">
         <v>73</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2126,9 +2198,9 @@
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="25"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="30"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="62"/>
+      <c r="D74" s="65"/>
       <c r="E74" s="3" t="s">
         <v>75</v>
       </c>
@@ -2141,9 +2213,9 @@
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="25"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="30"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="62"/>
+      <c r="D75" s="65"/>
       <c r="E75" s="3" t="s">
         <v>76</v>
       </c>
@@ -2154,9 +2226,9 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="25"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="30"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="62"/>
+      <c r="D76" s="65"/>
       <c r="E76" s="3" t="s">
         <v>77</v>
       </c>
@@ -2165,9 +2237,9 @@
       <c r="H76" s="3"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="25"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="30"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="62"/>
+      <c r="D77" s="65"/>
       <c r="E77" s="3" t="s">
         <v>78</v>
       </c>
@@ -2176,9 +2248,9 @@
       <c r="H77" s="3"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="25"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="31"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="63"/>
+      <c r="D78" s="66"/>
       <c r="E78" s="5" t="s">
         <v>51</v>
       </c>
@@ -2187,11 +2259,11 @@
       <c r="H78" s="3"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="42" t="s">
+      <c r="B79" s="46" t="s">
         <v>22</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="20" t="s">
+      <c r="D79" s="58" t="s">
         <v>104</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -2206,9 +2278,9 @@
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="43"/>
+      <c r="B80" s="47"/>
       <c r="C80" s="13"/>
-      <c r="D80" s="21"/>
+      <c r="D80" s="59"/>
       <c r="E80" s="6" t="s">
         <v>93</v>
       </c>
@@ -2221,9 +2293,9 @@
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="43"/>
+      <c r="B81" s="47"/>
       <c r="C81" s="13"/>
-      <c r="D81" s="21"/>
+      <c r="D81" s="59"/>
       <c r="E81" s="14" t="s">
         <v>59</v>
       </c>
@@ -2234,9 +2306,9 @@
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="43"/>
+      <c r="B82" s="47"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="21"/>
+      <c r="D82" s="59"/>
       <c r="E82" s="6" t="s">
         <v>60</v>
       </c>
@@ -2247,9 +2319,9 @@
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="43"/>
+      <c r="B83" s="47"/>
       <c r="C83" s="13"/>
-      <c r="D83" s="21"/>
+      <c r="D83" s="59"/>
       <c r="E83" s="6" t="s">
         <v>83</v>
       </c>
@@ -2260,9 +2332,9 @@
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="43"/>
+      <c r="B84" s="47"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="21"/>
+      <c r="D84" s="59"/>
       <c r="E84" s="6" t="s">
         <v>84</v>
       </c>
@@ -2273,9 +2345,9 @@
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="43"/>
+      <c r="B85" s="47"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="21"/>
+      <c r="D85" s="59"/>
       <c r="E85" s="6" t="s">
         <v>85</v>
       </c>
@@ -2284,9 +2356,9 @@
       <c r="H85" s="6"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="44"/>
+      <c r="B86" s="48"/>
       <c r="C86" s="13"/>
-      <c r="D86" s="45"/>
+      <c r="D86" s="60"/>
       <c r="E86" s="6" t="s">
         <v>86</v>
       </c>
@@ -2295,11 +2367,11 @@
       <c r="H86" s="6"/>
     </row>
     <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="40"/>
-      <c r="C87" s="70" t="s">
+      <c r="B87" s="56"/>
+      <c r="C87" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="D87" s="36" t="s">
+      <c r="D87" s="52" t="s">
         <v>79</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -2310,9 +2382,9 @@
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="41"/>
-      <c r="C88" s="71"/>
-      <c r="D88" s="37"/>
+      <c r="B88" s="57"/>
+      <c r="C88" s="55"/>
+      <c r="D88" s="53"/>
       <c r="E88" s="1" t="s">
         <v>81</v>
       </c>
@@ -2321,11 +2393,11 @@
       <c r="H88" s="1"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="49" t="s">
+      <c r="B89" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C89" s="50"/>
-      <c r="D89" s="46" t="s">
+      <c r="C89" s="49"/>
+      <c r="D89" s="32" t="s">
         <v>105</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -2336,9 +2408,9 @@
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="49"/>
-      <c r="C90" s="51"/>
-      <c r="D90" s="47"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="50"/>
+      <c r="D90" s="33"/>
       <c r="E90" s="1" t="s">
         <v>52</v>
       </c>
@@ -2347,9 +2419,9 @@
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="49"/>
-      <c r="C91" s="52"/>
-      <c r="D91" s="48"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="51"/>
+      <c r="D91" s="34"/>
       <c r="E91" s="2" t="s">
         <v>84</v>
       </c>
@@ -2374,15 +2446,22 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="B58:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D15:D30"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B79:B86"/>
+    <mergeCell ref="D79:D86"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="B87:B88"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C15:C30"/>
     <mergeCell ref="C3:D3"/>
@@ -2399,26 +2478,20 @@
     <mergeCell ref="D31:D39"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="B4:B54"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B79:B86"/>
-    <mergeCell ref="D79:D86"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="B58:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="C60:C65"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D15:D30"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización Guías CPH, Municipios, Organismos
</commit_message>
<xml_diff>
--- a/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
+++ b/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\menu\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUCIONES" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Iris Lechuga</author>
+    <author>DELL</author>
   </authors>
   <commentList>
     <comment ref="G72" authorId="0" shapeId="0">
@@ -54,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G87" authorId="0" shapeId="0">
+    <comment ref="G87" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,17 +65,41 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Iris Lechuga:</t>
+          <t xml:space="preserve">Iris Lechuga:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Estas Guías se quedan en el repositorio para consulta, no se suben a la plataforma </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G88" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-Estas Guías se quedan en el repositorio para consulta, no se suben a la plataforma </t>
+          <t xml:space="preserve">Iris Lechuga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Estas Guías se quedan en el repositorio para consulta, no se suben a la plataforma </t>
         </r>
       </text>
     </comment>
@@ -466,7 +491,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +542,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -694,150 +725,153 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -849,9 +883,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,39 +1166,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+    </row>
+    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="10" t="s">
         <v>98</v>
       </c>
@@ -1181,14 +1212,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="58" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1200,10 +1231,10 @@
       <c r="G4" s="12"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="39"/>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="26"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="59"/>
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1213,10 +1244,10 @@
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="47"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="40"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="26"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
@@ -1226,12 +1257,12 @@
       <c r="G6" s="15"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="43" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="26"/>
+      <c r="C7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1245,10 +1276,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="71"/>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="26"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1260,10 +1291,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="47"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="71"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="26"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
@@ -1275,10 +1306,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="71"/>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="26"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="6" t="s">
         <v>88</v>
       </c>
@@ -1290,10 +1321,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="71"/>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="26"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1305,12 +1336,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
-      <c r="C12" s="41" t="s">
+    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="26"/>
+      <c r="C12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1324,10 +1355,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="22"/>
+    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="26"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1339,10 +1370,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="22"/>
+    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1354,12 +1385,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
-      <c r="C15" s="28" t="s">
+    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="26"/>
+      <c r="C15" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1373,10 +1404,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="59"/>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="26"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1388,10 +1419,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="59"/>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="26"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1405,10 +1436,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="59"/>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="26"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1420,10 +1451,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="59"/>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="26"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1435,10 +1466,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="59"/>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="26"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1450,10 +1481,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="59"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="26"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1465,10 +1496,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="59"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="26"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1480,10 +1511,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="59"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="26"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1495,10 +1526,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="47"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="59"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="26"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1510,10 +1541,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="59"/>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="26"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1525,10 +1556,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="59"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="26"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="21"/>
       <c r="E26" s="6" t="s">
         <v>109</v>
       </c>
@@ -1540,10 +1571,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="47"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="59"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="26"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1555,10 +1586,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="47"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="59"/>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="26"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1570,10 +1601,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="47"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="59"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="26"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="6" t="s">
         <v>24</v>
       </c>
@@ -1585,10 +1616,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="47"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="59"/>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="26"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1600,12 +1631,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="47"/>
-      <c r="C31" s="23" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="26"/>
+      <c r="C31" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="23" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1619,10 +1650,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="47"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="22"/>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="26"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1634,10 +1665,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="47"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="22"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="26"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1649,10 +1680,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="47"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="22"/>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="26"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="3" t="s">
         <v>31</v>
       </c>
@@ -1664,10 +1695,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="47"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="22"/>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="26"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="3" t="s">
         <v>32</v>
       </c>
@@ -1679,10 +1710,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="47"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="22"/>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="26"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="3" t="s">
         <v>114</v>
       </c>
@@ -1692,10 +1723,10 @@
       <c r="G36" s="12"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="47"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="22"/>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="26"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="23"/>
       <c r="E37" s="3" t="s">
         <v>112</v>
       </c>
@@ -1705,10 +1736,10 @@
       <c r="G37" s="12"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="47"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="22"/>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="26"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="3" t="s">
         <v>113</v>
       </c>
@@ -1718,10 +1749,10 @@
       <c r="G38" s="12"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="47"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="22"/>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="26"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="23"/>
       <c r="E39" s="3" t="s">
         <v>90</v>
       </c>
@@ -1733,12 +1764,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="47"/>
-      <c r="C40" s="43" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="26"/>
+      <c r="C40" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="62" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
@@ -1750,10 +1781,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="47"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="44"/>
+    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="26"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="62"/>
       <c r="E41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1765,12 +1796,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="47"/>
-      <c r="C42" s="41" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="26"/>
+      <c r="C42" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -1782,10 +1813,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="47"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="22"/>
+    <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="26"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="23"/>
       <c r="E43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1795,10 +1826,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="47"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="22"/>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="26"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="23"/>
       <c r="E44" s="3" t="s">
         <v>42</v>
       </c>
@@ -1808,10 +1839,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="47"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="22"/>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="26"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="23"/>
       <c r="E45" s="3" t="s">
         <v>43</v>
       </c>
@@ -1821,10 +1852,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="47"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="22"/>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="26"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="23"/>
       <c r="E46" s="3" t="s">
         <v>44</v>
       </c>
@@ -1834,10 +1865,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="47"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="22"/>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="26"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="23"/>
       <c r="E47" s="3" t="s">
         <v>49</v>
       </c>
@@ -1847,10 +1878,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="47"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="22"/>
+    <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="26"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="23"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
       </c>
@@ -1860,10 +1891,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="47"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="22"/>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="26"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="23"/>
       <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
@@ -1873,10 +1904,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="47"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="22"/>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="26"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="23"/>
       <c r="E50" s="3" t="s">
         <v>47</v>
       </c>
@@ -1886,10 +1917,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="47"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="22"/>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="26"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="23"/>
       <c r="E51" s="3" t="s">
         <v>48</v>
       </c>
@@ -1899,10 +1930,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="47"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="22"/>
+    <row r="52" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B52" s="26"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="23"/>
       <c r="E52" s="4" t="s">
         <v>50</v>
       </c>
@@ -1912,12 +1943,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="47"/>
-      <c r="C53" s="43" t="s">
+    <row r="53" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="26"/>
+      <c r="C53" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="42" t="s">
+      <c r="D53" s="61" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -1929,10 +1960,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="48"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="42"/>
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="27"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="61"/>
       <c r="E54" s="7" t="s">
         <v>37</v>
       </c>
@@ -1942,14 +1973,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="19" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="32" t="s">
+      <c r="D55" s="36" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -1959,10 +1990,10 @@
       <c r="G55" s="12"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="19"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="33"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="39"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1970,10 +2001,10 @@
       <c r="G56" s="12"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="19"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="34"/>
+    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="39"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="38"/>
       <c r="E57" s="2" t="s">
         <v>56</v>
       </c>
@@ -1983,14 +2014,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="23" t="s">
+    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="67" t="s">
+      <c r="C58" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="D58" s="69" t="s">
+      <c r="D58" s="70" t="s">
         <v>58</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -2000,10 +2031,10 @@
       <c r="G58" s="12"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="23"/>
-      <c r="C59" s="68"/>
-      <c r="D59" s="70"/>
+    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="29"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="71"/>
       <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
@@ -2011,12 +2042,12 @@
       <c r="G59" s="12"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="23"/>
-      <c r="C60" s="23" t="s">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B60" s="29"/>
+      <c r="C60" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="23" t="s">
         <v>58</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2028,10 +2059,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="22"/>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="23"/>
       <c r="E61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2041,10 +2072,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="22"/>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="23"/>
       <c r="E62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2054,10 +2085,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="22"/>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="23"/>
       <c r="E63" s="3" t="s">
         <v>61</v>
       </c>
@@ -2067,10 +2098,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="23"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="22"/>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="23"/>
       <c r="E64" s="3" t="s">
         <v>22</v>
       </c>
@@ -2080,10 +2111,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="22"/>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="23"/>
       <c r="E65" s="3" t="s">
         <v>93</v>
       </c>
@@ -2093,12 +2124,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="23"/>
-      <c r="C66" s="23" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B66" s="29"/>
+      <c r="C66" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="D66" s="23" t="s">
         <v>58</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2108,10 +2139,10 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="23"/>
-      <c r="C67" s="23"/>
-      <c r="D67" s="22"/>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="23"/>
       <c r="E67" s="3" t="s">
         <v>65</v>
       </c>
@@ -2119,10 +2150,10 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="23"/>
-      <c r="C68" s="23"/>
-      <c r="D68" s="22"/>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="23"/>
       <c r="E68" s="3" t="s">
         <v>66</v>
       </c>
@@ -2130,10 +2161,10 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="22"/>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="23"/>
       <c r="E69" s="3" t="s">
         <v>67</v>
       </c>
@@ -2141,10 +2172,10 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="23"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="22"/>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="23"/>
       <c r="E70" s="3" t="s">
         <v>68</v>
       </c>
@@ -2152,14 +2183,14 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="19" t="s">
+    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D71" s="24" t="s">
+      <c r="D71" s="66" t="s">
         <v>70</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -2169,10 +2200,10 @@
       <c r="G71" s="12"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="19"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="25"/>
+    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="39"/>
+      <c r="C72" s="65"/>
+      <c r="D72" s="67"/>
       <c r="E72" s="2" t="s">
         <v>71</v>
       </c>
@@ -2180,90 +2211,90 @@
       <c r="G72" s="15"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="23" t="s">
+    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="61"/>
-      <c r="D73" s="64" t="s">
+      <c r="C73" s="30"/>
+      <c r="D73" s="33" t="s">
         <v>73</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
+      <c r="G73" s="12"/>
       <c r="H73" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="23"/>
-      <c r="C74" s="62"/>
-      <c r="D74" s="65"/>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B74" s="29"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="34"/>
       <c r="E74" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G74" s="3"/>
+      <c r="G74" s="12"/>
       <c r="H74" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="23"/>
-      <c r="C75" s="62"/>
-      <c r="D75" s="65"/>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" s="29"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="34"/>
       <c r="E75" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G75" s="3"/>
+      <c r="G75" s="12"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="23"/>
-      <c r="C76" s="62"/>
-      <c r="D76" s="65"/>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B76" s="29"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="34"/>
       <c r="E76" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
+      <c r="G76" s="12"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="23"/>
-      <c r="C77" s="62"/>
-      <c r="D77" s="65"/>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B77" s="29"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="34"/>
       <c r="E77" s="3" t="s">
         <v>78</v>
       </c>
       <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
+      <c r="G77" s="12"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="23"/>
-      <c r="C78" s="63"/>
-      <c r="D78" s="66"/>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B78" s="29"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="35"/>
       <c r="E78" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
+      <c r="G78" s="12"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="46" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="58" t="s">
+      <c r="D79" s="20" t="s">
         <v>104</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -2277,10 +2308,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="47"/>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B80" s="26"/>
       <c r="C80" s="13"/>
-      <c r="D80" s="59"/>
+      <c r="D80" s="21"/>
       <c r="E80" s="6" t="s">
         <v>93</v>
       </c>
@@ -2292,10 +2323,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="47"/>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B81" s="26"/>
       <c r="C81" s="13"/>
-      <c r="D81" s="59"/>
+      <c r="D81" s="21"/>
       <c r="E81" s="14" t="s">
         <v>59</v>
       </c>
@@ -2305,10 +2336,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="47"/>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B82" s="26"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="59"/>
+      <c r="D82" s="21"/>
       <c r="E82" s="6" t="s">
         <v>60</v>
       </c>
@@ -2318,10 +2349,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="47"/>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B83" s="26"/>
       <c r="C83" s="13"/>
-      <c r="D83" s="59"/>
+      <c r="D83" s="21"/>
       <c r="E83" s="6" t="s">
         <v>83</v>
       </c>
@@ -2331,10 +2362,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="47"/>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B84" s="26"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="59"/>
+      <c r="D84" s="21"/>
       <c r="E84" s="6" t="s">
         <v>84</v>
       </c>
@@ -2344,10 +2375,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="47"/>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B85" s="26"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="59"/>
+      <c r="D85" s="21"/>
       <c r="E85" s="6" t="s">
         <v>85</v>
       </c>
@@ -2355,10 +2386,10 @@
       <c r="G85" s="12"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="48"/>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B86" s="27"/>
       <c r="C86" s="13"/>
-      <c r="D86" s="60"/>
+      <c r="D86" s="28"/>
       <c r="E86" s="6" t="s">
         <v>86</v>
       </c>
@@ -2366,38 +2397,38 @@
       <c r="G86" s="12"/>
       <c r="H86" s="6"/>
     </row>
-    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="56"/>
-      <c r="C87" s="54" t="s">
+    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="47"/>
+      <c r="C87" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="D87" s="52" t="s">
+      <c r="D87" s="43" t="s">
         <v>79</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
+      <c r="G87" s="12"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="57"/>
-      <c r="C88" s="55"/>
-      <c r="D88" s="53"/>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B88" s="48"/>
+      <c r="C88" s="46"/>
+      <c r="D88" s="44"/>
       <c r="E88" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
+      <c r="G88" s="12"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="19" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B89" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="C89" s="49"/>
-      <c r="D89" s="32" t="s">
+      <c r="C89" s="40"/>
+      <c r="D89" s="36" t="s">
         <v>105</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -2407,29 +2438,29 @@
       <c r="G89" s="12"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="19"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="33"/>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B90" s="39"/>
+      <c r="C90" s="41"/>
+      <c r="D90" s="37"/>
       <c r="E90" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
+      <c r="G90" s="12"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="19"/>
-      <c r="C91" s="51"/>
-      <c r="D91" s="34"/>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B91" s="39"/>
+      <c r="C91" s="42"/>
+      <c r="D91" s="38"/>
       <c r="E91" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
+      <c r="G91" s="12"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B92" s="17" t="s">
         <v>116</v>
       </c>
@@ -2446,22 +2477,17 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D15:D30"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B79:B86"/>
-    <mergeCell ref="D79:D86"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="D73:D78"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="B58:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C15:C30"/>
     <mergeCell ref="C3:D3"/>
@@ -2478,17 +2504,22 @@
     <mergeCell ref="D31:D39"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="B4:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="B58:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="C60:C65"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B79:B86"/>
+    <mergeCell ref="D79:D86"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D15:D30"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
actualización matriz de guías
</commit_message>
<xml_diff>
--- a/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
+++ b/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github Repositorio\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\menu\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUCIONES" sheetId="1" r:id="rId1"/>
@@ -26,36 +26,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Iris Lechuga</author>
     <author>DELL</author>
   </authors>
   <commentList>
-    <comment ref="G72" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Iris Lechuga:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Guía pendiente 
-Aun no se sabe su si va a usar DCCP </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G87" authorId="1" shapeId="0">
+    <comment ref="G87" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G88" authorId="1" shapeId="0">
+    <comment ref="G88" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +465,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,12 +503,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -681,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -715,7 +683,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -725,21 +692,147 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -757,132 +850,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1166,39 +1133,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+    </row>
+    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="10" t="s">
         <v>98</v>
       </c>
@@ -1212,14 +1179,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="57" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1231,10 +1198,10 @@
       <c r="G4" s="12"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="51"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="43"/>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="25"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1244,25 +1211,25 @@
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="51"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="44"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="25"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="51"/>
-      <c r="C7" s="47" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="25"/>
+      <c r="C7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1276,10 +1243,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="71"/>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="25"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1291,10 +1258,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="51"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="71"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="25"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
@@ -1306,10 +1273,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="71"/>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="25"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="6" t="s">
         <v>88</v>
       </c>
@@ -1321,10 +1288,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="71"/>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="25"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1336,9 +1303,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
-      <c r="C12" s="45" t="s">
+    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="25"/>
+      <c r="C12" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="22" t="s">
@@ -1355,9 +1322,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="45"/>
+    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="25"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="4" t="s">
         <v>10</v>
@@ -1370,9 +1337,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="22"/>
       <c r="E14" s="4" t="s">
         <v>7</v>
@@ -1385,12 +1352,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="51"/>
-      <c r="C15" s="32" t="s">
+    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="25"/>
+      <c r="C15" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1404,10 +1371,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="63"/>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="25"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1419,10 +1386,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="63"/>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="25"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1436,10 +1403,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="51"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="63"/>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="25"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1451,10 +1418,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="51"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="63"/>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="25"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1466,10 +1433,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="51"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="63"/>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="25"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1481,10 +1448,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="51"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="63"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="25"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1496,10 +1463,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="51"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="63"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="25"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1511,10 +1478,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="51"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="63"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="25"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1526,10 +1493,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="51"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="63"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="25"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1541,10 +1508,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="51"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="63"/>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="25"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1556,10 +1523,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="51"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="63"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="25"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="6" t="s">
         <v>109</v>
       </c>
@@ -1571,10 +1538,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="51"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="63"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="25"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1586,10 +1553,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="51"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="63"/>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="25"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1601,10 +1568,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="51"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="63"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="25"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="6" t="s">
         <v>24</v>
       </c>
@@ -1616,10 +1583,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="51"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="63"/>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="25"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1631,9 +1598,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="51"/>
-      <c r="C31" s="23" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="25"/>
+      <c r="C31" s="28" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="22" t="s">
@@ -1650,9 +1617,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="51"/>
-      <c r="C32" s="23"/>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="25"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="22"/>
       <c r="E32" s="3" t="s">
         <v>29</v>
@@ -1665,9 +1632,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="51"/>
-      <c r="C33" s="23"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="25"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="22"/>
       <c r="E33" s="3" t="s">
         <v>30</v>
@@ -1680,9 +1647,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="51"/>
-      <c r="C34" s="23"/>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="25"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="22"/>
       <c r="E34" s="3" t="s">
         <v>31</v>
@@ -1690,14 +1657,14 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="15"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="51"/>
-      <c r="C35" s="23"/>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="25"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="22"/>
       <c r="E35" s="3" t="s">
         <v>32</v>
@@ -1710,9 +1677,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="51"/>
-      <c r="C36" s="23"/>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="25"/>
+      <c r="C36" s="28"/>
       <c r="D36" s="22"/>
       <c r="E36" s="3" t="s">
         <v>114</v>
@@ -1723,9 +1690,9 @@
       <c r="G36" s="12"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="51"/>
-      <c r="C37" s="23"/>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="25"/>
+      <c r="C37" s="28"/>
       <c r="D37" s="22"/>
       <c r="E37" s="3" t="s">
         <v>112</v>
@@ -1736,9 +1703,9 @@
       <c r="G37" s="12"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="51"/>
-      <c r="C38" s="23"/>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="25"/>
+      <c r="C38" s="28"/>
       <c r="D38" s="22"/>
       <c r="E38" s="3" t="s">
         <v>113</v>
@@ -1749,9 +1716,9 @@
       <c r="G38" s="12"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="51"/>
-      <c r="C39" s="23"/>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="25"/>
+      <c r="C39" s="28"/>
       <c r="D39" s="22"/>
       <c r="E39" s="3" t="s">
         <v>90</v>
@@ -1764,12 +1731,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="51"/>
-      <c r="C40" s="47" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="25"/>
+      <c r="C40" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="48" t="s">
+      <c r="D40" s="61" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
@@ -1781,10 +1748,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="51"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="48"/>
+    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="25"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="61"/>
       <c r="E41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1796,9 +1763,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="51"/>
-      <c r="C42" s="45" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="25"/>
+      <c r="C42" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="22" t="s">
@@ -1813,9 +1780,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="51"/>
-      <c r="C43" s="45"/>
+    <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
+      <c r="C43" s="23"/>
       <c r="D43" s="22"/>
       <c r="E43" s="4" t="s">
         <v>41</v>
@@ -1826,9 +1793,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="51"/>
-      <c r="C44" s="45"/>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="25"/>
+      <c r="C44" s="23"/>
       <c r="D44" s="22"/>
       <c r="E44" s="3" t="s">
         <v>42</v>
@@ -1839,9 +1806,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="51"/>
-      <c r="C45" s="45"/>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="25"/>
+      <c r="C45" s="23"/>
       <c r="D45" s="22"/>
       <c r="E45" s="3" t="s">
         <v>43</v>
@@ -1852,9 +1819,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="51"/>
-      <c r="C46" s="45"/>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="25"/>
+      <c r="C46" s="23"/>
       <c r="D46" s="22"/>
       <c r="E46" s="3" t="s">
         <v>44</v>
@@ -1865,9 +1832,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="51"/>
-      <c r="C47" s="45"/>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="25"/>
+      <c r="C47" s="23"/>
       <c r="D47" s="22"/>
       <c r="E47" s="3" t="s">
         <v>49</v>
@@ -1878,9 +1845,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="51"/>
-      <c r="C48" s="45"/>
+    <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="25"/>
+      <c r="C48" s="23"/>
       <c r="D48" s="22"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
@@ -1891,9 +1858,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="51"/>
-      <c r="C49" s="45"/>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="25"/>
+      <c r="C49" s="23"/>
       <c r="D49" s="22"/>
       <c r="E49" s="3" t="s">
         <v>46</v>
@@ -1904,9 +1871,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="51"/>
-      <c r="C50" s="45"/>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="25"/>
+      <c r="C50" s="23"/>
       <c r="D50" s="22"/>
       <c r="E50" s="3" t="s">
         <v>47</v>
@@ -1917,9 +1884,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="51"/>
-      <c r="C51" s="45"/>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="25"/>
+      <c r="C51" s="23"/>
       <c r="D51" s="22"/>
       <c r="E51" s="3" t="s">
         <v>48</v>
@@ -1930,9 +1897,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="51"/>
-      <c r="C52" s="45"/>
+    <row r="52" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B52" s="25"/>
+      <c r="C52" s="23"/>
       <c r="D52" s="22"/>
       <c r="E52" s="4" t="s">
         <v>50</v>
@@ -1943,12 +1910,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="51"/>
-      <c r="C53" s="47" t="s">
+    <row r="53" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="25"/>
+      <c r="C53" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="46" t="s">
+      <c r="D53" s="60" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -1960,10 +1927,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="52"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="46"/>
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="26"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="60"/>
       <c r="E54" s="7" t="s">
         <v>37</v>
       </c>
@@ -1973,14 +1940,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="19" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="D55" s="35" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -1990,10 +1957,10 @@
       <c r="G55" s="12"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="19"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="37"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="38"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="36"/>
       <c r="E56" s="1" t="s">
         <v>51</v>
       </c>
@@ -2001,10 +1968,10 @@
       <c r="G56" s="12"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="19"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="38"/>
+    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="38"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="2" t="s">
         <v>56</v>
       </c>
@@ -2014,14 +1981,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="23" t="s">
+    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="D58" s="28" t="s">
+      <c r="D58" s="69" t="s">
         <v>58</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -2033,10 +2000,10 @@
       <c r="G58" s="12"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="23"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="29"/>
+    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="28"/>
+      <c r="C59" s="68"/>
+      <c r="D59" s="70"/>
       <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
@@ -2046,9 +2013,9 @@
       <c r="G59" s="12"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="23"/>
-      <c r="C60" s="23" t="s">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B60" s="28"/>
+      <c r="C60" s="28" t="s">
         <v>11</v>
       </c>
       <c r="D60" s="22" t="s">
@@ -2065,9 +2032,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
       <c r="D61" s="22"/>
       <c r="E61" s="3" t="s">
         <v>59</v>
@@ -2080,9 +2047,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
       <c r="D62" s="22"/>
       <c r="E62" s="3" t="s">
         <v>60</v>
@@ -2095,9 +2062,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
       <c r="D63" s="22"/>
       <c r="E63" s="3" t="s">
         <v>61</v>
@@ -2110,9 +2077,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="23"/>
-      <c r="C64" s="23"/>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
       <c r="D64" s="22"/>
       <c r="E64" s="3" t="s">
         <v>22</v>
@@ -2125,9 +2092,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
       <c r="D65" s="22"/>
       <c r="E65" s="3" t="s">
         <v>93</v>
@@ -2140,9 +2107,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="23"/>
-      <c r="C66" s="23" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B66" s="28"/>
+      <c r="C66" s="28" t="s">
         <v>63</v>
       </c>
       <c r="D66" s="22" t="s">
@@ -2157,9 +2124,9 @@
       <c r="G66" s="12"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="23"/>
-      <c r="C67" s="23"/>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
       <c r="D67" s="22"/>
       <c r="E67" s="3" t="s">
         <v>65</v>
@@ -2170,9 +2137,9 @@
       <c r="G67" s="12"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="23"/>
-      <c r="C68" s="23"/>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
       <c r="D68" s="22"/>
       <c r="E68" s="3" t="s">
         <v>66</v>
@@ -2183,9 +2150,9 @@
       <c r="G68" s="12"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
       <c r="D69" s="22"/>
       <c r="E69" s="3" t="s">
         <v>67</v>
@@ -2196,9 +2163,9 @@
       <c r="G69" s="12"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="23"/>
-      <c r="C70" s="23"/>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
       <c r="D70" s="22"/>
       <c r="E70" s="3" t="s">
         <v>68</v>
@@ -2209,14 +2176,14 @@
       <c r="G70" s="12"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="19" t="s">
+    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="D71" s="24" t="s">
+      <c r="D71" s="65" t="s">
         <v>70</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -2226,23 +2193,23 @@
       <c r="G71" s="12"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="19"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="25"/>
+    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="38"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="66"/>
       <c r="E72" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F72" s="1"/>
-      <c r="G72" s="15"/>
+      <c r="G72" s="12"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="23" t="s">
+    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="65"/>
-      <c r="D73" s="68" t="s">
+      <c r="C73" s="29"/>
+      <c r="D73" s="32" t="s">
         <v>73</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2254,10 +2221,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="23"/>
-      <c r="C74" s="66"/>
-      <c r="D74" s="69"/>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B74" s="28"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="33"/>
       <c r="E74" s="3" t="s">
         <v>75</v>
       </c>
@@ -2269,10 +2236,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="23"/>
-      <c r="C75" s="66"/>
-      <c r="D75" s="69"/>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" s="28"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="33"/>
       <c r="E75" s="3" t="s">
         <v>76</v>
       </c>
@@ -2282,10 +2249,10 @@
       <c r="G75" s="12"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="23"/>
-      <c r="C76" s="66"/>
-      <c r="D76" s="69"/>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B76" s="28"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="33"/>
       <c r="E76" s="3" t="s">
         <v>77</v>
       </c>
@@ -2293,10 +2260,10 @@
       <c r="G76" s="12"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="23"/>
-      <c r="C77" s="66"/>
-      <c r="D77" s="69"/>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B77" s="28"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="33"/>
       <c r="E77" s="3" t="s">
         <v>78</v>
       </c>
@@ -2304,10 +2271,10 @@
       <c r="G77" s="12"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="23"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="70"/>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B78" s="28"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="34"/>
       <c r="E78" s="5" t="s">
         <v>51</v>
       </c>
@@ -2315,12 +2282,12 @@
       <c r="G78" s="12"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="50" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="62" t="s">
+      <c r="D79" s="19" t="s">
         <v>104</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -2334,10 +2301,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="51"/>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B80" s="25"/>
       <c r="C80" s="13"/>
-      <c r="D80" s="63"/>
+      <c r="D80" s="20"/>
       <c r="E80" s="6" t="s">
         <v>93</v>
       </c>
@@ -2349,10 +2316,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="51"/>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B81" s="25"/>
       <c r="C81" s="13"/>
-      <c r="D81" s="63"/>
+      <c r="D81" s="20"/>
       <c r="E81" s="14" t="s">
         <v>59</v>
       </c>
@@ -2362,10 +2329,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="51"/>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B82" s="25"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="63"/>
+      <c r="D82" s="20"/>
       <c r="E82" s="6" t="s">
         <v>60</v>
       </c>
@@ -2375,10 +2342,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="51"/>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B83" s="25"/>
       <c r="C83" s="13"/>
-      <c r="D83" s="63"/>
+      <c r="D83" s="20"/>
       <c r="E83" s="6" t="s">
         <v>83</v>
       </c>
@@ -2388,10 +2355,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="51"/>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B84" s="25"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="63"/>
+      <c r="D84" s="20"/>
       <c r="E84" s="6" t="s">
         <v>84</v>
       </c>
@@ -2401,10 +2368,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="51"/>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B85" s="25"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="63"/>
+      <c r="D85" s="20"/>
       <c r="E85" s="6" t="s">
         <v>85</v>
       </c>
@@ -2412,10 +2379,10 @@
       <c r="G85" s="12"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="52"/>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B86" s="26"/>
       <c r="C86" s="13"/>
-      <c r="D86" s="64"/>
+      <c r="D86" s="27"/>
       <c r="E86" s="6" t="s">
         <v>86</v>
       </c>
@@ -2423,12 +2390,12 @@
       <c r="G86" s="12"/>
       <c r="H86" s="6"/>
     </row>
-    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="60"/>
-      <c r="C87" s="58" t="s">
+    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="46"/>
+      <c r="C87" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D87" s="56" t="s">
+      <c r="D87" s="42" t="s">
         <v>79</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -2438,10 +2405,10 @@
       <c r="G87" s="12"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="61"/>
-      <c r="C88" s="59"/>
-      <c r="D88" s="57"/>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B88" s="47"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="43"/>
       <c r="E88" s="1" t="s">
         <v>81</v>
       </c>
@@ -2449,12 +2416,12 @@
       <c r="G88" s="12"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="19" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B89" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C89" s="53"/>
-      <c r="D89" s="36" t="s">
+      <c r="C89" s="39"/>
+      <c r="D89" s="35" t="s">
         <v>105</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -2464,10 +2431,10 @@
       <c r="G89" s="12"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="19"/>
-      <c r="C90" s="54"/>
-      <c r="D90" s="37"/>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B90" s="38"/>
+      <c r="C90" s="40"/>
+      <c r="D90" s="36"/>
       <c r="E90" s="1" t="s">
         <v>52</v>
       </c>
@@ -2475,10 +2442,10 @@
       <c r="G90" s="12"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="19"/>
-      <c r="C91" s="55"/>
-      <c r="D91" s="38"/>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B91" s="38"/>
+      <c r="C91" s="41"/>
+      <c r="D91" s="37"/>
       <c r="E91" s="2" t="s">
         <v>84</v>
       </c>
@@ -2486,12 +2453,12 @@
       <c r="G91" s="12"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="17" t="s">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B92" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C92" s="18"/>
-      <c r="D92" s="16" t="s">
+      <c r="C92" s="17"/>
+      <c r="D92" s="15" t="s">
         <v>117</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -2503,22 +2470,17 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D15:D30"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B79:B86"/>
-    <mergeCell ref="D79:D86"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="D73:D78"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="B58:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C15:C30"/>
     <mergeCell ref="C3:D3"/>
@@ -2535,17 +2497,22 @@
     <mergeCell ref="D31:D39"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="B4:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="B58:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="C60:C65"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B79:B86"/>
+    <mergeCell ref="D79:D86"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D15:D30"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Coeficiente PEF Guía de Uso
</commit_message>
<xml_diff>
--- a/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
+++ b/PDRMYE/16 GUÍAS DE USUARIO/Matriz de guias/Matriz de guias.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\menu\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\PDRMYE\16 GUÍAS DE USUARIO\Matriz de guias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUCIONES" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="119">
   <si>
     <t>GUÍA RÁPIDA DE OPERACIONES DE LA PLATAFORMA DE DISTRIBUCIÓN DE RECURSOS A MUNICIPIOS Y ORGANISMOS PÚBLICOS DESCENTRALIZADOS MÓDULO “COORDINACIÓN DE PLANEACIÓN HACENDARÍA</t>
   </si>
@@ -695,21 +695,147 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -727,132 +853,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1137,38 +1137,38 @@
   <dimension ref="B2:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+      <selection activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="52.33203125" customWidth="1"/>
-    <col min="5" max="5" width="53.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-    </row>
-    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+    </row>
+    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="10" t="s">
         <v>98</v>
       </c>
@@ -1182,14 +1182,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="49" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="57" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1203,10 +1203,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="50"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="42"/>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="25"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1218,10 +1218,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="50"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="43"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="25"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
@@ -1231,12 +1231,12 @@
       <c r="G6" s="12"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
-      <c r="C7" s="46" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1250,10 +1250,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="50"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="70"/>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1265,10 +1265,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="50"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="70"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
@@ -1280,10 +1280,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="50"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="70"/>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="6" t="s">
         <v>88</v>
       </c>
@@ -1295,10 +1295,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="50"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="70"/>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1310,12 +1310,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="50"/>
-      <c r="C12" s="44" t="s">
+    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="25"/>
+      <c r="C12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1329,10 +1329,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="50"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="21"/>
+    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="25"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1344,10 +1344,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="50"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="21"/>
+    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="50"/>
-      <c r="C15" s="31" t="s">
+    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1378,10 +1378,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="50"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="62"/>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1393,10 +1393,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="50"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="62"/>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="25"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1410,10 +1410,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="50"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="62"/>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="25"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1425,10 +1425,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="50"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="62"/>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1440,10 +1440,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="50"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="62"/>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1455,10 +1455,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="50"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="62"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="25"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1470,10 +1470,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="50"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="62"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1485,10 +1485,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="50"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="62"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1500,10 +1500,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="50"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="62"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="25"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1515,10 +1515,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="50"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="62"/>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1530,10 +1530,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="50"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="62"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="25"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="6" t="s">
         <v>109</v>
       </c>
@@ -1545,10 +1545,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="50"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="62"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="25"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1560,10 +1560,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="50"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="62"/>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="25"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1575,10 +1575,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="50"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="62"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="25"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="6" t="s">
         <v>24</v>
       </c>
@@ -1590,10 +1590,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="50"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="62"/>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="25"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1605,12 +1605,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="50"/>
-      <c r="C31" s="22" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="25"/>
+      <c r="C31" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1624,10 +1624,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="50"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="21"/>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="25"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1639,10 +1639,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="50"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="21"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="25"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1654,10 +1654,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="50"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="21"/>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="25"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="3" t="s">
         <v>31</v>
       </c>
@@ -1669,10 +1669,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="50"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="21"/>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="25"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="3" t="s">
         <v>32</v>
       </c>
@@ -1684,10 +1684,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="50"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="21"/>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="25"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="3" t="s">
         <v>114</v>
       </c>
@@ -1695,12 +1695,14 @@
         <v>107</v>
       </c>
       <c r="G36" s="12"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="50"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="21"/>
+      <c r="H36" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="25"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="3" t="s">
         <v>112</v>
       </c>
@@ -1708,12 +1710,14 @@
         <v>107</v>
       </c>
       <c r="G37" s="12"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="50"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="21"/>
+      <c r="H37" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="25"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="3" t="s">
         <v>113</v>
       </c>
@@ -1721,12 +1725,14 @@
         <v>107</v>
       </c>
       <c r="G38" s="12"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="50"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="21"/>
+      <c r="H38" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="25"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="3" t="s">
         <v>90</v>
       </c>
@@ -1738,12 +1744,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="50"/>
-      <c r="C40" s="46" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="25"/>
+      <c r="C40" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="47" t="s">
+      <c r="D40" s="61" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
@@ -1755,10 +1761,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="50"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="47"/>
+    <row r="41" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="25"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="61"/>
       <c r="E41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1770,12 +1776,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="50"/>
-      <c r="C42" s="44" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="25"/>
+      <c r="C42" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -1787,10 +1793,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B43" s="50"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="21"/>
+    <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="25"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1800,10 +1806,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="50"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="21"/>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="25"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="3" t="s">
         <v>42</v>
       </c>
@@ -1813,10 +1819,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="50"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="21"/>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="25"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="3" t="s">
         <v>43</v>
       </c>
@@ -1826,10 +1832,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="50"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="21"/>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="25"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="22"/>
       <c r="E46" s="3" t="s">
         <v>44</v>
       </c>
@@ -1839,10 +1845,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="50"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="21"/>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="25"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="22"/>
       <c r="E47" s="3" t="s">
         <v>49</v>
       </c>
@@ -1852,10 +1858,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" s="50"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="21"/>
+    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="25"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="22"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
       </c>
@@ -1865,10 +1871,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="50"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="21"/>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="25"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
@@ -1878,10 +1884,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="50"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="21"/>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="25"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="3" t="s">
         <v>47</v>
       </c>
@@ -1891,10 +1897,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="50"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="21"/>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="25"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="22"/>
       <c r="E51" s="3" t="s">
         <v>48</v>
       </c>
@@ -1904,10 +1910,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B52" s="50"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="21"/>
+    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="25"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="22"/>
       <c r="E52" s="4" t="s">
         <v>50</v>
       </c>
@@ -1917,12 +1923,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="50"/>
-      <c r="C53" s="46" t="s">
+    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="25"/>
+      <c r="C53" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="45" t="s">
+      <c r="D53" s="60" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -1934,10 +1940,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="51"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="45"/>
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="26"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="60"/>
       <c r="E54" s="7" t="s">
         <v>37</v>
       </c>
@@ -1947,11 +1953,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="18" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="62" t="s">
         <v>95</v>
       </c>
       <c r="D55" s="35" t="s">
@@ -1966,9 +1972,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B56" s="18"/>
-      <c r="C56" s="48"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="38"/>
+      <c r="C56" s="63"/>
       <c r="D56" s="36"/>
       <c r="E56" s="1" t="s">
         <v>51</v>
@@ -1979,9 +1985,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="18"/>
-      <c r="C57" s="20"/>
+    <row r="57" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="38"/>
+      <c r="C57" s="64"/>
       <c r="D57" s="37"/>
       <c r="E57" s="2" t="s">
         <v>56</v>
@@ -1992,14 +1998,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="22" t="s">
+    <row r="58" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="25" t="s">
+      <c r="C58" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="D58" s="27" t="s">
+      <c r="D58" s="69" t="s">
         <v>58</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -2013,10 +2019,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="22"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="28"/>
+    <row r="59" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="28"/>
+      <c r="C59" s="68"/>
+      <c r="D59" s="70"/>
       <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
@@ -2028,12 +2034,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B60" s="22"/>
-      <c r="C60" s="22" t="s">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="28"/>
+      <c r="C60" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D60" s="22" t="s">
         <v>58</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2047,10 +2053,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="21"/>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="22"/>
       <c r="E61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2062,10 +2068,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="21"/>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="22"/>
       <c r="E62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2077,10 +2083,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B63" s="22"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="21"/>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="22"/>
       <c r="E63" s="3" t="s">
         <v>61</v>
       </c>
@@ -2092,10 +2098,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B64" s="22"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="21"/>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="22"/>
       <c r="E64" s="3" t="s">
         <v>22</v>
       </c>
@@ -2107,10 +2113,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="21"/>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="22"/>
       <c r="E65" s="3" t="s">
         <v>93</v>
       </c>
@@ -2122,12 +2128,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B66" s="22"/>
-      <c r="C66" s="22" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="28"/>
+      <c r="C66" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="21" t="s">
+      <c r="D66" s="22" t="s">
         <v>58</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2137,12 +2143,14 @@
         <v>107</v>
       </c>
       <c r="G66" s="12"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="21"/>
+      <c r="H66" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="22"/>
       <c r="E67" s="3" t="s">
         <v>65</v>
       </c>
@@ -2150,12 +2158,14 @@
         <v>107</v>
       </c>
       <c r="G67" s="12"/>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="21"/>
+      <c r="H67" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="22"/>
       <c r="E68" s="3" t="s">
         <v>66</v>
       </c>
@@ -2163,12 +2173,14 @@
         <v>107</v>
       </c>
       <c r="G68" s="12"/>
-      <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="21"/>
+      <c r="H68" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="22"/>
       <c r="E69" s="3" t="s">
         <v>67</v>
       </c>
@@ -2176,12 +2188,14 @@
         <v>107</v>
       </c>
       <c r="G69" s="12"/>
-      <c r="H69" s="3"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="21"/>
+      <c r="H69" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="22"/>
       <c r="E70" s="3" t="s">
         <v>68</v>
       </c>
@@ -2189,16 +2203,18 @@
         <v>107</v>
       </c>
       <c r="G70" s="12"/>
-      <c r="H70" s="3"/>
-    </row>
-    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="18" t="s">
+      <c r="H70" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="D71" s="23" t="s">
+      <c r="D71" s="65" t="s">
         <v>70</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -2210,10 +2226,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="18"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="24"/>
+    <row r="72" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="38"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="66"/>
       <c r="E72" s="2" t="s">
         <v>71</v>
       </c>
@@ -2223,12 +2239,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="22" t="s">
+    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="64"/>
-      <c r="D73" s="67" t="s">
+      <c r="C73" s="29"/>
+      <c r="D73" s="32" t="s">
         <v>73</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2240,10 +2256,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B74" s="22"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="68"/>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="28"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="33"/>
       <c r="E74" s="3" t="s">
         <v>75</v>
       </c>
@@ -2255,10 +2271,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B75" s="22"/>
-      <c r="C75" s="65"/>
-      <c r="D75" s="68"/>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="28"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="33"/>
       <c r="E75" s="3" t="s">
         <v>76</v>
       </c>
@@ -2270,10 +2286,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B76" s="22"/>
-      <c r="C76" s="65"/>
-      <c r="D76" s="68"/>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="28"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="33"/>
       <c r="E76" s="3" t="s">
         <v>77</v>
       </c>
@@ -2283,10 +2299,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B77" s="22"/>
-      <c r="C77" s="65"/>
-      <c r="D77" s="68"/>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="28"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="33"/>
       <c r="E77" s="3" t="s">
         <v>78</v>
       </c>
@@ -2296,10 +2312,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B78" s="22"/>
-      <c r="C78" s="66"/>
-      <c r="D78" s="69"/>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="28"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="34"/>
       <c r="E78" s="5" t="s">
         <v>51</v>
       </c>
@@ -2309,12 +2325,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B79" s="49" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="61" t="s">
+      <c r="D79" s="19" t="s">
         <v>104</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -2328,10 +2344,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B80" s="50"/>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="25"/>
       <c r="C80" s="13"/>
-      <c r="D80" s="62"/>
+      <c r="D80" s="20"/>
       <c r="E80" s="6" t="s">
         <v>93</v>
       </c>
@@ -2343,10 +2359,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B81" s="50"/>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="25"/>
       <c r="C81" s="13"/>
-      <c r="D81" s="62"/>
+      <c r="D81" s="20"/>
       <c r="E81" s="14" t="s">
         <v>59</v>
       </c>
@@ -2356,10 +2372,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B82" s="50"/>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="25"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="62"/>
+      <c r="D82" s="20"/>
       <c r="E82" s="6" t="s">
         <v>60</v>
       </c>
@@ -2369,10 +2385,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B83" s="50"/>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="25"/>
       <c r="C83" s="13"/>
-      <c r="D83" s="62"/>
+      <c r="D83" s="20"/>
       <c r="E83" s="6" t="s">
         <v>83</v>
       </c>
@@ -2382,10 +2398,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B84" s="50"/>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="25"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="62"/>
+      <c r="D84" s="20"/>
       <c r="E84" s="6" t="s">
         <v>84</v>
       </c>
@@ -2395,34 +2411,38 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B85" s="50"/>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="25"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="62"/>
+      <c r="D85" s="20"/>
       <c r="E85" s="6" t="s">
         <v>85</v>
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="12"/>
-      <c r="H85" s="6"/>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B86" s="51"/>
+      <c r="H85" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="26"/>
       <c r="C86" s="13"/>
-      <c r="D86" s="63"/>
+      <c r="D86" s="27"/>
       <c r="E86" s="6" t="s">
         <v>86</v>
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="12"/>
-      <c r="H86" s="6"/>
-    </row>
-    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="59"/>
-      <c r="C87" s="57" t="s">
+      <c r="H86" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="46"/>
+      <c r="C87" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D87" s="55" t="s">
+      <c r="D87" s="42" t="s">
         <v>79</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -2434,10 +2454,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B88" s="60"/>
-      <c r="C88" s="58"/>
-      <c r="D88" s="56"/>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="47"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="43"/>
       <c r="E88" s="1" t="s">
         <v>81</v>
       </c>
@@ -2447,11 +2467,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B89" s="18" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C89" s="52"/>
+      <c r="C89" s="39"/>
       <c r="D89" s="35" t="s">
         <v>105</v>
       </c>
@@ -2464,9 +2484,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B90" s="18"/>
-      <c r="C90" s="53"/>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="38"/>
+      <c r="C90" s="40"/>
       <c r="D90" s="36"/>
       <c r="E90" s="1" t="s">
         <v>52</v>
@@ -2477,9 +2497,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B91" s="18"/>
-      <c r="C91" s="54"/>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="38"/>
+      <c r="C91" s="41"/>
       <c r="D91" s="37"/>
       <c r="E91" s="2" t="s">
         <v>84</v>
@@ -2488,7 +2508,7 @@
       <c r="G91" s="12"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="16" t="s">
         <v>116</v>
       </c>
@@ -2505,22 +2525,17 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D15:D30"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B79:B86"/>
-    <mergeCell ref="D79:D86"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="D73:D78"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="B58:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C15:C30"/>
     <mergeCell ref="C3:D3"/>
@@ -2537,17 +2552,22 @@
     <mergeCell ref="D31:D39"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="B4:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="B58:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="C60:C65"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B79:B86"/>
+    <mergeCell ref="D79:D86"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D15:D30"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>